<commit_message>
add cardboard box processing, change tests and assortment processing
</commit_message>
<xml_diff>
--- a/Projects/PEPSICOUK/Tests/Data/test_case_1.xlsx
+++ b/Projects/PEPSICOUK/Tests/Data/test_case_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="matches" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,15 +14,17 @@
     <sheet name="stitch_groups" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$N$52</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$P$52</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$U$12</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$P$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">matches!$A$1:$N$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">matches!$A$1:$P$52</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">matches!$A$1:$N$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">matches!$A$1:$N$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">matches!$A$1:$P$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">matches!$A$1:$N$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">matches!$A$1:$P$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">matches!$A$1:$N$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">matches!$A$1:$N$52</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$N$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">matches!$A$1:$N$52</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">scif!$A$1:$U$12</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
   <si>
     <t xml:space="preserve">probe_match_fk</t>
   </si>
@@ -138,6 +140,9 @@
     <t xml:space="preserve">Hero</t>
   </si>
   <si>
+    <t xml:space="preserve">form_factor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Product 1</t>
   </si>
   <si>
@@ -178,6 +183,9 @@
   </si>
   <si>
     <t xml:space="preserve">Non-pepsico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cardboard box</t>
   </si>
   <si>
     <t xml:space="preserve">General Empty</t>
@@ -578,29 +586,29 @@
   </sheetPr>
   <dimension ref="A1:Q52"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="bottomLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.5714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="4.45408163265306"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.515306122449"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="4.32142857142857"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="16.3316326530612"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2826,7 +2834,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N52"/>
+  <autoFilter ref="A1:P52"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2843,29 +2851,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.8928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.3673469387755"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="25.1632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="4.59183673469388"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2914,6 +2922,9 @@
       <c r="O1" s="22" t="s">
         <v>33</v>
       </c>
+      <c r="P1" s="22" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -2923,16 +2934,16 @@
         <v>10</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>136</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>2</v>
@@ -2941,13 +2952,13 @@
         <v>2</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2958,16 +2969,16 @@
         <v>5</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>136</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>2</v>
@@ -2976,13 +2987,13 @@
         <v>2</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2993,16 +3004,16 @@
         <v>15</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>189</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>2</v>
@@ -3011,13 +3022,13 @@
         <v>2</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3028,10 +3039,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>2</v>
@@ -3040,10 +3051,13 @@
         <v>3</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3054,10 +3068,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>0</v>
@@ -3066,7 +3080,7 @@
         <v>1</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3077,10 +3091,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>2</v>
@@ -3089,10 +3103,10 @@
         <v>2</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3111,28 +3125,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q16" activeCellId="0" sqref="Q16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V6" activeCellId="0" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.4642857142857"/>
-    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.0612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.1938775510204"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="20" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3143,25 +3157,25 @@
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>21</v>
@@ -3198,6 +3212,9 @@
       </c>
       <c r="U1" s="2" t="s">
         <v>32</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3227,10 +3244,10 @@
         <v>1</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J2" s="0" t="str">
         <f aca="false">VLOOKUP(B2,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3272,6 +3289,10 @@
         <f aca="false">VLOOKUP($B2, all_products!$A$2:$N$6, 14, 0)</f>
         <v>0</v>
       </c>
+      <c r="V2" s="0" t="n">
+        <f aca="false">VLOOKUP($B2, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
@@ -3300,10 +3321,10 @@
         <v>1</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J3" s="0" t="str">
         <f aca="false">VLOOKUP(B3,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3345,6 +3366,10 @@
         <f aca="false">VLOOKUP($B3, all_products!$A$2:$N$6, 14, 0)</f>
         <v>EAT REAL HUMMUS LENTIL &amp; QUINOA CHIPS</v>
       </c>
+      <c r="V3" s="0" t="n">
+        <f aca="false">VLOOKUP($B3, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
@@ -3373,10 +3398,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J4" s="0" t="str">
         <f aca="false">VLOOKUP(B4,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3418,6 +3443,10 @@
         <f aca="false">VLOOKUP($B4, all_products!$A$2:$N$6, 14, 0)</f>
         <v>0</v>
       </c>
+      <c r="V4" s="0" t="n">
+        <f aca="false">VLOOKUP($B4, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
@@ -3446,10 +3475,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J5" s="0" t="str">
         <f aca="false">VLOOKUP(B5,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3491,6 +3520,10 @@
         <f aca="false">VLOOKUP($B5, all_products!$A$2:$N$6, 14, 0)</f>
         <v>0</v>
       </c>
+      <c r="V5" s="0" t="n">
+        <f aca="false">VLOOKUP($B5, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -3519,10 +3552,10 @@
         <v>1</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J6" s="0" t="str">
         <f aca="false">VLOOKUP(B6,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3564,6 +3597,10 @@
         <f aca="false">VLOOKUP($B6, all_products!$A$2:$N$6, 14, 0)</f>
         <v>0</v>
       </c>
+      <c r="V6" s="0" t="str">
+        <f aca="false">VLOOKUP($B6, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>cardboard box</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -3592,10 +3629,10 @@
         <v>1</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J7" s="0" t="str">
         <f aca="false">VLOOKUP(B7,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3637,6 +3674,10 @@
         <f aca="false">VLOOKUP($B7, all_products!$A$2:$N$6, 14, 0)</f>
         <v>EAT REAL HUMMUS LENTIL &amp; QUINOA CHIPS</v>
       </c>
+      <c r="V7" s="0" t="n">
+        <f aca="false">VLOOKUP($B7, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -3665,10 +3706,10 @@
         <v>1</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J8" s="0" t="str">
         <f aca="false">VLOOKUP(B8,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3710,6 +3751,10 @@
         <f aca="false">VLOOKUP($B8, all_products!$A$2:$N$6, 14, 0)</f>
         <v>0</v>
       </c>
+      <c r="V8" s="0" t="n">
+        <f aca="false">VLOOKUP($B8, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -3738,10 +3783,10 @@
         <v>1</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J9" s="0" t="str">
         <f aca="false">VLOOKUP(B9,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3783,6 +3828,10 @@
         <f aca="false">VLOOKUP($B9, all_products!$A$2:$N$6, 14, 0)</f>
         <v>0</v>
       </c>
+      <c r="V9" s="0" t="n">
+        <f aca="false">VLOOKUP($B9, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -3811,10 +3860,10 @@
         <v>2</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J10" s="0" t="str">
         <f aca="false">VLOOKUP(B10,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3856,6 +3905,10 @@
         <f aca="false">VLOOKUP($B10, all_products!$A$2:$N$6, 14, 0)</f>
         <v>EAT REAL HUMMUS LENTIL &amp; QUINOA CHIPS</v>
       </c>
+      <c r="V10" s="0" t="n">
+        <f aca="false">VLOOKUP($B10, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -3884,10 +3937,10 @@
         <v>2</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J11" s="0" t="str">
         <f aca="false">VLOOKUP(B11,all_products!$A$2:$C$6, 3, 0)</f>
@@ -3929,6 +3982,10 @@
         <f aca="false">VLOOKUP($B11, all_products!$A$2:$N$6, 14, 0)</f>
         <v>0</v>
       </c>
+      <c r="V11" s="0" t="n">
+        <f aca="false">VLOOKUP($B11, all_products!$A$2:$P$6, 16, 0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
@@ -3957,10 +4014,10 @@
         <v>2</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="J12" s="0" t="str">
         <f aca="false">VLOOKUP(B12,all_products!$A$2:$C$6, 3, 0)</f>
@@ -4000,6 +4057,10 @@
       </c>
       <c r="U12" s="0" t="n">
         <f aca="false">VLOOKUP($B12, all_products!$A$2:$N$6, 14, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="V12" s="0" t="n">
+        <f aca="false">VLOOKUP($B12, all_products!$A$2:$P$6, 16, 0)</f>
         <v>0</v>
       </c>
     </row>
@@ -4029,7 +4090,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4037,7 +4098,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>